<commit_message>
saving more data, improved plotting, added thermometer some renames of execs
</commit_message>
<xml_diff>
--- a/csv_automation/temperature_profiles.xlsx
+++ b/csv_automation/temperature_profiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Home Directory/Programming/Automation/csv_automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0E4460-3AEE-544E-8C89-2CA688A9AE20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42918575-19D5-EF47-97F8-85672B9822B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temperature_profiles" sheetId="1" r:id="rId1"/>
@@ -1072,10 +1072,10 @@
   <dimension ref="A1:Z136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1785,10 +1785,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="K12">
         <v>0.5</v>
@@ -1815,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="S12">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="T12">
         <v>2</v>
@@ -1833,10 +1833,10 @@
         <v>13</v>
       </c>
       <c r="I13">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="K13">
         <v>0.5</v>
@@ -1863,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="S13">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="T13">
         <v>2</v>
@@ -1881,10 +1881,10 @@
         <v>14</v>
       </c>
       <c r="I14">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="K14">
         <v>0.5</v>
@@ -1911,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="S14">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="T14">
         <v>2</v>

</xml_diff>